<commit_message>
Final Report update in the git repo
</commit_message>
<xml_diff>
--- a/accuracy_scores.xlsx
+++ b/accuracy_scores.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>SVC</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>AdaBoost</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>k5</t>
+  </si>
+  <si>
+    <t>est 300</t>
+  </si>
+  <si>
+    <t>depth 3</t>
   </si>
 </sst>
 </file>
@@ -563,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I25"/>
+  <dimension ref="B1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1095,6 +1107,26 @@
         <v>0.70109999999999995</v>
       </c>
     </row>
+    <row r="26" spans="2:9">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26">
+        <v>0.92989999999999995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>